<commit_message>
fgix: WIP - Add DTO validation and serialization tests
</commit_message>
<xml_diff>
--- a/tests/C2Pro_Test_Suites_Master.xlsx
+++ b/tests/C2Pro_Test_Suites_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esus_\Documents\AI\ZTWQ\c2pro\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20574B73-32BB-4CF4-A1E6-7B37358BA636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA186636-5833-4748-8EC2-640B38F3A73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suite Test" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3410" uniqueCount="862">
   <si>
     <t>Nº</t>
   </si>
@@ -2917,6 +2917,293 @@
 3.  **GREEN:** Generate `src/core/security/*.py`. Use "Fake It" pattern.
 4.  **UPDATE:** Remind me to update `C2PRO_TDD_BACKLOG_v1.0.md`.
 **AWAITING INPUT:** Please provide a TS-UC-SEC ID.</t>
+  </si>
+  <si>
+    <t> Orden | Agente | Tests | Sprint | Bloquea | Crítico |</t>
+  </si>
+  <si>
+    <t>|-------|--------|-------|--------|---------|---------|</t>
+  </si>
+  <si>
+    <t>| 1 | Agente 10 (DTOs) | 40 | S1 | Todos | ✅ |</t>
+  </si>
+  <si>
+    <t>| 2 | Agente 1 (Security) | 156 | S1-S2 | Todos | ✅ |</t>
+  </si>
+  <si>
+    <t>| 3 | Agente 8 (Event Bus básico) | 34 | S2 | Async flows | ✅ |</t>
+  </si>
+  <si>
+    <t>| 4 | Agente 2 (Documents) | 162 | S3-S4 | Analysis, Coherence | ✅ |</t>
+  </si>
+  <si>
+    <t>| 5 | Agente 6 (Coherence) | 206 | S5-S6 | Dashboard, E2E | 🔴 CRÍTICO |</t>
+  </si>
+  <si>
+    <t>| 6 | Agente 3 (Projects) | 116 | S7 | Procurement | ⚠️ |</t>
+  </si>
+  <si>
+    <t>| 7 | Agente 4 (Procurement) | 116 | S8 | Coherence rules | ⚠️ |</t>
+  </si>
+  <si>
+    <t>| 8 | Agente 7 (Stakeholders) | 112 | S9 | RACI | ⚠️ |</t>
+  </si>
+  <si>
+    <t>| 9 | Agente 5 (Analysis) | 78 | S10 | Graph RAG | ⚠️ |</t>
+  </si>
+  <si>
+    <t>| 10 | Agente 9 (Observability) | 68 | S11 | Monitoring | ⚠️ |</t>
+  </si>
+  <si>
+    <t>| 11 | Agente 11 (Integration) | 184 | S11-S12 | E2E | ✅ |</t>
+  </si>
+  <si>
+    <t>| 12 | Agente 10 (HTTP) | 62 | S12 | API | ⚠️ |</t>
+  </si>
+  <si>
+    <t>| 13 | Agente 8 (Celery/DLQ) | 44 | S12 | Workers | ⚠️ |</t>
+  </si>
+  <si>
+    <t>| 14 | Agente 12 (E2E) | 78 | S13-S14 | Release | ✅ |</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 1 - SECURITY CORE SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **Security Lead**.
+* **CRITICAL:** Read `agents.md`. Enforce "4-Layer Security" model.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **MCP Gateway:** `TS-UC-SEC-MCP-001` to `004` (Allowlist, Rate Limit, Query Limits, Audit).
+* **Anonymizer:** `TS-UC-SEC-ANO-001` to `003` (PII Detection, Strategies, Config).
+* **Isolation:** `TS-UC-SEC-TNT-001` (Tenant Context).
+* **Auth:** `TS-UC-SEC-JWT-001` (JWT Validation).
+* **Audit:** `TS-UC-SEC-AUD-001` (Core Trail).
+* **Gaming:** `TS-UC-SEC-GAM-001` (Detection Logic).
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if the test exists. If yes, validate strict security assertions. If no, generate the test (RED).
+2.  **RED:** Confirm failure (e.g., "Unauthorized Access" or "PII Leak").
+3.  **GREEN:** Implement minimal logic in `src/core/security` or `src/core/auth`. Use "Fake It" pattern initially.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-UC-SEC ID.</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 2 - DOCUMENTS DOMAIN SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **Documents Module Lead**.
+* **CRITICAL:** Read `agents.md`. `Clause` entity is the Single Source of Truth.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **Clauses:** `TS-UD-DOC-CLS-001` to `003` (Entity, Types, Hierarchy).
+* **Entities:** `TS-UD-DOC-ENT-001` to `004` (Dates, Money, Durations, Stakeholders).
+* **Document:** `TS-UD-DOC-DOC-001` (Entity) &amp; `TS-UD-DOC-CNF-001` (Confidence).
+* **Use Cases:** `TS-UA-DOC-UC-*` (Upload, Extract).
+* **Services:** `TS-UA-SVC-EXT-*` (Extraction Services).
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Ensure Domain Entities are pure Pydantic.
+2.  **RED:** Generate test in `tests/modules/documents/domain`. Assert validation failure.
+3.  **GREEN:** Implement logic in `src/modules/documents/domain`. No DB imports allowed.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-UD-DOC ID.</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 3 - PROJECTS &amp; WBS SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **Projects Module Lead**.
+* **CRITICAL:** Read `agents.md`. Focus on Recursive Hierarchies.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **WBS Logic:** `TS-UD-PRJ-WBS-001` to `004` (Entity, Hierarchy, Validation, CRUD).
+* **Project:** `TS-UD-PRJ-PRJ-001` (Entity).
+* **Contracts:** `TS-UD-PRJ-DTO-001` (DTOs &amp; Ports for Integration).
+* **Use Cases:** `TS-UA-PRJ-UC-*` (Generate WBS).
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Verify recursive parent/child logic tests.
+2.  **RED:** Generate test in `tests/modules/projects`. Assert hierarchy constraint failure.
+3.  **GREEN:** Implement logic in `src/modules/projects`. Ensure strictly typed relationships.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-UD-PRJ ID.</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 4 - PROCUREMENT LOGIC SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **Procurement Module Lead**.
+* **CRITICAL:** Read `agents.md`. Focus on Lead Time Logic.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **BOM:** `TS-UD-PROC-BOM-001` &amp; `002` (Entity, Validation).
+* **Lead Time:** `TS-UD-PROC-LTM-001` to `004` (Calc, Incoterms, Customs, Alerts).
+* **Planning:** `TS-UD-PROC-PLN-001` (Plan Generation).
+* **Use Cases:** `TS-UA-PROC-UC-*` (Generate BOM, Calc LTM).
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Verify math/date calculation assertions.
+2.  **RED:** Generate test in `tests/modules/procurement`. Assert wrong date calculation.
+3.  **GREEN:** Implement logic in `src/modules/procurement`. Use standard `datetime` libs.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-UD-PROC ID.</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 5 - ANALYSIS &amp; GRAPH SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **Analysis Module Lead**.
+* **CRITICAL:** Read `agents.md`. Focus on Graph Consistency.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **Alerts:** `TS-UD-ANA-ALR-001` (Entity).
+* **Graph:** `TS-UD-ANA-GRP-001` &amp; `002` (Node, Relationship).
+* **Search:** `TS-UD-ANA-SRC-001` &amp; `HYB-001` (Semantic, Hybrid).
+* **Use Cases:** `TS-UA-ANA-UC-*`.
+* **Neo4j:** `TS-INT-GRP-NEO-001` (Integration Adapter).
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Ensure Node/Edge properties are validated.
+2.  **RED:** Generate test in `tests/modules/analysis`. Assert missing graph label/property.
+3.  **GREEN:** Implement logic in `src/modules/analysis`. Mock Neo4j driver in unit tests.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-UD-ANA ID.</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 6 - COHERENCE ENGINE SPECIALIST (CRITICAL)
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **Coherence Module Lead**.
+* **CRITICAL:** Read `agents.md`. Adhere to the 6-Category Model (SCOPE, BUDGET, TIME, TECH, LEGAL, QUALITY).
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **Setup:** `TS-UD-COH-CAT-001` (Enums/Weights).
+* **Rules:** `TS-UD-COH-RUL-001` to `006` (All Categories).
+* **Scoring:** `TS-UD-COH-SCR-001` to `003` (Calculator).
+* **Gaming:** `TS-UD-COH-GAM-001` (Anti-Gaming Policy).
+* **Mapping:** `TS-UD-COH-ALR-001` (Alert Mapping).
+* **Use Cases:** `TS-UA-COH-UC-*`.
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Verify logic for specific Rules (e.g., R11, R6).
+2.  **RED:** Generate test in `tests/modules/coherence`. Assert score calculation error.
+3.  **GREEN:** Implement logic in `src/modules/coherence`. Use pure functions for rules.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-UD-COH ID.</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 7 - STAKEHOLDERS SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **Stakeholders Module Lead**.
+* **CRITICAL:** Read `agents.md`.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **Entities:** `TS-UD-STK-ENT-001` &amp; `MAP-001`.
+* **Classification:** `TS-UD-STK-CLS-001` &amp; `002` (Power/Interest).
+* **RACI:** `TS-UD-STK-RAC-001` to `003` (Matrix Generation).
+* **Use Cases:** `TS-UA-STK-UC-*`.
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Verify RACI matrix dimensions/roles.
+2.  **RED:** Generate test in `tests/modules/stakeholders`. Assert invalid RACI assignment.
+3.  **GREEN:** Implement logic in `src/modules/stakeholders`.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-UD-STK ID.</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 8 - ASYNC ARCHITECTURE SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **Async Infrastructure Lead**.
+* **CRITICAL:** Read `agents.md`.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **Event Bus:** `TS-INT-EVT-BUS-001` (Redis Pub/Sub).
+* **Celery:** `TS-INT-EVT-CEL-001` (Jobs).
+* **Resilience:** `TS-INT-EVT-DLQ-001` (Dead Letter Queue).
+* **E2E Async:** `TS-E2E-*` (Specific async flows).
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Use `pytest-asyncio` and `testcontainers`.
+2.  **RED:** Generate test in `tests/infrastructure/events`. Assert message not received.
+3.  **GREEN:** Implement adapters in `src/core/events` or `src/adapters`.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-INT-EVT ID.</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 9 - OBSERVABILITY SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **Observability Lead**.
+* **CRITICAL:** Read `agents.md`.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **Budget:** `TS-UA-SVC-BDG-001` (Tracking &amp; Circuit Breaker).
+* **Logging/Tracing:** Tests related to `core/observability` (mapped to generic infra suites or implicitly required).
+* **Monitoring:** Dashboard Data Logic.
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Verify Structlog/OpenTelemetry mocks.
+2.  **RED:** Generate test asserting missing trace_id or budget overflow.
+3.  **GREEN:** Implement interceptors/services in `src/core/observability`.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a ID (e.g., TS-UA-SVC-BDG-001).</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 10 - API CONTRACTS SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **API Layer Lead**.
+* **CRITICAL:** Read `agents.md`. Routers must be THIN.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **DTOs:** `TS-UA-DTO-ALL-001` &amp; `SER-001` (Validation).
+* **HTTP:** `TS-UAD-HTTP-RTR-001` (Routers).
+* **Middleware:** `TS-UAD-HTTP-MDW-001` (Auth/Tenant).
+* **Errors:** `TS-UAD-HTTP-ERR-001` (Handlers).
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Verify serialization and HTTP codes.
+2.  **RED:** Generate test using `TestClient`. Assert 400/404/422 responses.
+3.  **GREEN:** Implement Routers/DTOs in `src/.../adapters/http` or `application/dtos`.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-UA-DTO or TS-UAD-HTTP ID.</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 11 - INTEGRATION SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **Integration Architect**.
+* **CRITICAL:** Read `agents.md`. Verify Boundaries.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **Cross-Module:** `TS-INT-MOD-WBS-001`, `DOC-001`, `ANA-001`, `STK-001`.
+* **External:** `TS-INT-EXT-LLM-001/002` (LLM Clients).
+* **Database:** `TS-INT-DB-*` (Repositories) &amp; `TS-INT-GRP-NEO-001`.
+* **Adapters:** `TS-UAD-PER-*` (Persistence Generic).
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Use `Testcontainers` for DB tests.
+2.  **RED:** Generate integration test ensuring data persistence or event flow.
+3.  **GREEN:** Implement Repositories or Integration Adapters.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-INT ID.</t>
+  </si>
+  <si>
+    <t>**SYSTEM ROLE:** AGENT 12 - QA &amp; E2E SPECIALIST
+**1. INITIALIZATION &amp; CONTEXT**
+You are the **QA Lead**.
+* **CRITICAL:** Read `agents.md`. Test the full system.
+* **LATENCY:** Output code directly.
+**2. ASSIGNED SCOPE (100% Match with Index)**
+You are responsible for the following components and Suite IDs:
+* **Flows:** `TS-E2E-FLW-DOC`, `ALR`, `BLK` (Business Flows).
+* **Security E2E:** `TS-E2E-SEC-TNT`, `MCP`.
+* **Errors:** `TS-E2E-ERR-TIM`, `CON`, `REC` (Resilience).
+* **Perf:** `TS-E2E-PER-LRG` (Performance).
+**3. EXECUTION PROTOCOL (SMART TDD)**
+1.  **ANALYZE:** Check if test exists. Simulate real user journeys.
+2.  **RED:** Generate E2E script (Pytest/Playwright). Assert flow completion.
+3.  **GREEN:** Fix underlying system issues or adjust logic to pass E2E.
+4.  **UPDATE:** Request update for `C2PRO_TDD_BACKLOG_v1.0.md`.
+**AWAITING INPUT:** Provide a TS-E2E ID.</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>claude</t>
   </si>
 </sst>
 </file>
@@ -2982,7 +3269,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3004,6 +3291,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3081,7 +3374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3129,8 +3422,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3438,12 +3738,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A114" sqref="A114"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L83" sqref="L83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="19.149999999999999" customHeight="1"/>
@@ -3455,7 +3754,7 @@
     <col min="11" max="11" width="62.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.149999999999999" customHeight="1">
+    <row r="1" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3489,8 +3788,11 @@
       <c r="K1" s="3" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+      <c r="L1" s="20" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3525,7 +3827,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="3" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3560,7 +3862,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="4" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3595,7 +3897,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="5" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3630,7 +3932,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="6" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3665,7 +3967,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="7" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3700,7 +4002,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="8" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3735,7 +4037,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="9" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3770,7 +4072,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="10" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3805,7 +4107,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="11" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -3840,7 +4142,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="12" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -3875,7 +4177,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="13" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3910,7 +4212,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="14" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -3942,7 +4244,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="15" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -3974,7 +4276,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="16" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -4009,7 +4311,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="17" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -4041,7 +4343,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="18" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -4070,7 +4372,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="19" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -4099,7 +4401,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="20" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -4128,7 +4430,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="21" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -4157,7 +4459,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="22" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -4186,7 +4488,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="23" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -4221,7 +4523,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="24" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -4253,7 +4555,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="25" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -4282,7 +4584,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="26" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -4311,7 +4613,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="27" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -4340,7 +4642,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="28" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -4375,7 +4677,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="29" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -4404,7 +4706,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="30" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -4433,7 +4735,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="31" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -4462,7 +4764,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="32" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -4491,7 +4793,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="33" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -4520,7 +4822,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="34" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -4552,7 +4854,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="35" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -4584,7 +4886,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="36" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -4616,7 +4918,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="37" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -4648,7 +4950,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="38" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -4680,7 +4982,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="39" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -4715,7 +5017,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="40" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -4744,7 +5046,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="41" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -4773,7 +5075,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="42" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -4802,7 +5104,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="43" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -4831,7 +5133,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="44" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -4860,7 +5162,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="45" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -4889,7 +5191,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="46" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -4918,7 +5220,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="47" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -4953,7 +5255,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="48" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -4982,7 +5284,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="49" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -5011,7 +5313,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="50" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -5040,7 +5342,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="51" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -5069,7 +5371,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="52" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -5098,7 +5400,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="53" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -5127,7 +5429,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="54" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -5156,7 +5458,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="55" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -5185,7 +5487,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="56" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -5214,7 +5516,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="57" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -5243,7 +5545,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="58" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -5272,7 +5574,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="59" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -5301,7 +5603,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="60" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -5330,7 +5632,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="61" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -5359,7 +5661,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="62" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -5388,7 +5690,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="63" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -5417,7 +5719,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="64" spans="1:9" ht="19.149999999999999" customHeight="1">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -5446,7 +5748,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="65" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -5475,7 +5777,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="66" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -5504,7 +5806,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="67" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -5533,7 +5835,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="68" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -5562,7 +5864,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="69" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A69" t="s">
         <v>73</v>
       </c>
@@ -5591,7 +5893,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="70" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -5620,7 +5922,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="71" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -5649,7 +5951,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="72" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -5684,7 +5986,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="73" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -5719,7 +6021,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="74" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -5754,7 +6056,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="75" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -5786,7 +6088,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="76" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -5815,7 +6117,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="77" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A77" t="s">
         <v>81</v>
       </c>
@@ -5850,7 +6152,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="78" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -5952,24 +6254,24 @@
         <v>802</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="81" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B81" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="C81" t="s">
-        <v>311</v>
+        <v>326</v>
       </c>
       <c r="D81" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E81" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="F81" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G81" t="s">
         <v>407</v>
@@ -5980,28 +6282,25 @@
       <c r="I81" t="s">
         <v>381</v>
       </c>
-      <c r="J81" s="2" t="s">
-        <v>380</v>
-      </c>
       <c r="K81" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="82" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B82" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="C82" t="s">
-        <v>312</v>
+        <v>327</v>
       </c>
       <c r="D82" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E82" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F82" t="s">
         <v>353</v>
@@ -6016,7 +6315,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="83" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -6050,25 +6349,28 @@
       <c r="K83" s="2" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+      <c r="L83" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B84" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="C84" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
       <c r="D84" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E84" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="F84" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G84" t="s">
         <v>407</v>
@@ -6080,7 +6382,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="85" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A85" t="s">
         <v>89</v>
       </c>
@@ -6112,24 +6414,24 @@
         <v>794</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="86" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C86" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D86" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E86" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F86" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G86" t="s">
         <v>407</v>
@@ -6144,7 +6446,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="87" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -6173,24 +6475,24 @@
         <v>381</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="88" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A88" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B88" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C88" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D88" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E88" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F88" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G88" t="s">
         <v>407</v>
@@ -6202,24 +6504,24 @@
         <v>381</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="89" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B89" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C89" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D89" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E89" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F89" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G89" t="s">
         <v>407</v>
@@ -6231,7 +6533,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="90" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A90" t="s">
         <v>94</v>
       </c>
@@ -6266,7 +6568,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="91" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -6298,7 +6600,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="92" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -6330,7 +6632,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="93" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A93" t="s">
         <v>97</v>
       </c>
@@ -6359,7 +6661,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="94" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A94" t="s">
         <v>98</v>
       </c>
@@ -6391,7 +6693,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="95" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A95" t="s">
         <v>99</v>
       </c>
@@ -6426,21 +6728,21 @@
         <v>408</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="96" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A96" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B96" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C96" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="D96" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E96" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F96" t="s">
         <v>353</v>
@@ -6455,24 +6757,24 @@
         <v>381</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="97" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B97" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="C97" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="D97" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E97" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F97" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G97" t="s">
         <v>407</v>
@@ -6483,22 +6785,28 @@
       <c r="I97" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+      <c r="J97" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="L97" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B98" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="C98" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="D98" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E98" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F98" t="s">
         <v>353</v>
@@ -6512,8 +6820,11 @@
       <c r="I98" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+      <c r="L98" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A99" t="s">
         <v>103</v>
       </c>
@@ -6545,7 +6856,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="100" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A100" t="s">
         <v>104</v>
       </c>
@@ -6577,7 +6888,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="101" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A101" t="s">
         <v>105</v>
       </c>
@@ -6606,7 +6917,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="102" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -6638,7 +6949,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="103" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -6673,7 +6984,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="104" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A104" t="s">
         <v>108</v>
       </c>
@@ -6702,7 +7013,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="105" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A105" t="s">
         <v>109</v>
       </c>
@@ -6830,7 +7141,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="109" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A109" t="s">
         <v>113</v>
       </c>
@@ -6865,7 +7176,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="110" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A110" t="s">
         <v>114</v>
       </c>
@@ -6900,7 +7211,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="111" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A111" t="s">
         <v>115</v>
       </c>
@@ -6935,7 +7246,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="112" spans="1:12" ht="19.149999999999999" customHeight="1">
       <c r="A112" t="s">
         <v>116</v>
       </c>
@@ -6964,7 +7275,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="19.149999999999999" hidden="1" customHeight="1">
+    <row r="113" spans="1:11" ht="19.149999999999999" customHeight="1">
       <c r="A113" t="s">
         <v>117</v>
       </c>
@@ -7027,9 +7338,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J114" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters blank="1"/>
-    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A81:J98">
+      <sortCondition ref="B1:B114"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7071,12 +7382,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FEA767-FEF3-4D23-9143-13AEAC680DA5}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P404"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A320" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G318" sqref="G318:G331"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7117,7 +7427,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="2" spans="1:9" ht="31.5" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>119</v>
       </c>
@@ -7142,7 +7452,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="3" spans="1:9" ht="31.5" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>119</v>
       </c>
@@ -7167,7 +7477,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="4" spans="1:9" ht="31.5" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>119</v>
       </c>
@@ -7192,7 +7502,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="46.5" hidden="1" thickBot="1">
+    <row r="5" spans="1:9" ht="46.5" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>119</v>
       </c>
@@ -7217,7 +7527,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="6" spans="1:9" ht="31.5" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>119</v>
       </c>
@@ -7242,7 +7552,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="7" spans="1:9" ht="31.5" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>119</v>
       </c>
@@ -7267,7 +7577,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="8" spans="1:9" ht="31.5" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>119</v>
       </c>
@@ -7292,7 +7602,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="9" spans="1:9" ht="31.5" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>119</v>
       </c>
@@ -7317,7 +7627,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="10" spans="1:9" ht="31.5" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>119</v>
       </c>
@@ -7342,7 +7652,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="11" spans="1:9" ht="31.5" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>119</v>
       </c>
@@ -7367,7 +7677,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="12" spans="1:9" ht="31.5" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>119</v>
       </c>
@@ -7392,7 +7702,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="13" spans="1:9" ht="31.5" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>119</v>
       </c>
@@ -7417,7 +7727,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="14" spans="1:9" ht="31.5" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>119</v>
       </c>
@@ -7442,7 +7752,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="15" spans="1:9" ht="31.5" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>119</v>
       </c>
@@ -7467,7 +7777,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="31.5" hidden="1" thickBot="1">
+    <row r="16" spans="1:9" ht="31.5" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>119</v>
       </c>
@@ -7492,7 +7802,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="17" spans="1:16" ht="31.5" thickBot="1">
       <c r="A17" s="6" t="s">
         <v>119</v>
       </c>
@@ -7517,7 +7827,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="46.5" hidden="1" thickBot="1">
+    <row r="18" spans="1:16" ht="46.5" thickBot="1">
       <c r="A18" s="6" t="s">
         <v>119</v>
       </c>
@@ -7542,7 +7852,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="19" spans="1:16" ht="31.5" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>119</v>
       </c>
@@ -7567,7 +7877,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="20" spans="1:16" ht="31.5" thickBot="1">
       <c r="A20" s="6" t="s">
         <v>119</v>
       </c>
@@ -7592,7 +7902,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="21" spans="1:16" ht="31.5" thickBot="1">
       <c r="A21" s="6" t="s">
         <v>119</v>
       </c>
@@ -7617,7 +7927,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="22" spans="1:16" ht="31.5" thickBot="1">
       <c r="A22" s="6" t="s">
         <v>119</v>
       </c>
@@ -7642,7 +7952,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="23" spans="1:16" ht="31.5" thickBot="1">
       <c r="A23" s="6" t="s">
         <v>119</v>
       </c>
@@ -7667,7 +7977,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="24" spans="1:16" ht="31.5" thickBot="1">
       <c r="A24" s="6" t="s">
         <v>120</v>
       </c>
@@ -7699,7 +8009,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="25" spans="1:16" ht="31.5" thickBot="1">
       <c r="A25" s="6" t="s">
         <v>120</v>
       </c>
@@ -7731,7 +8041,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="26" spans="1:16" ht="31.5" thickBot="1">
       <c r="A26" s="6" t="s">
         <v>120</v>
       </c>
@@ -7763,7 +8073,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="27" spans="1:16" ht="31.5" thickBot="1">
       <c r="A27" s="6" t="s">
         <v>120</v>
       </c>
@@ -7795,7 +8105,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="28" spans="1:16" ht="31.5" thickBot="1">
       <c r="A28" s="6" t="s">
         <v>120</v>
       </c>
@@ -7827,7 +8137,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="29" spans="1:16" ht="31.5" thickBot="1">
       <c r="A29" s="6" t="s">
         <v>120</v>
       </c>
@@ -7859,7 +8169,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="30" spans="1:16" ht="31.5" thickBot="1">
       <c r="A30" s="6" t="s">
         <v>120</v>
       </c>
@@ -7891,7 +8201,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="31" spans="1:16" ht="31.5" thickBot="1">
       <c r="A31" s="6" t="s">
         <v>120</v>
       </c>
@@ -7923,7 +8233,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="32" spans="1:16" ht="31.5" thickBot="1">
       <c r="A32" s="6" t="s">
         <v>120</v>
       </c>
@@ -7955,7 +8265,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="33" spans="1:16" ht="31.5" thickBot="1">
       <c r="A33" s="6" t="s">
         <v>120</v>
       </c>
@@ -7987,7 +8297,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="34" spans="1:16" ht="31.5" thickBot="1">
       <c r="A34" s="6" t="s">
         <v>120</v>
       </c>
@@ -8019,7 +8329,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="35" spans="1:16" ht="31.5" thickBot="1">
       <c r="A35" s="6" t="s">
         <v>120</v>
       </c>
@@ -8051,7 +8361,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="36" spans="1:16" ht="31.5" thickBot="1">
       <c r="A36" s="6" t="s">
         <v>120</v>
       </c>
@@ -8083,7 +8393,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="37" spans="1:16" ht="31.5" thickBot="1">
       <c r="A37" s="6" t="s">
         <v>120</v>
       </c>
@@ -8115,7 +8425,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="38" spans="1:16" ht="31.5" thickBot="1">
       <c r="A38" s="6" t="s">
         <v>120</v>
       </c>
@@ -8147,7 +8457,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="39" spans="1:16" ht="31.5" thickBot="1">
       <c r="A39" s="6" t="s">
         <v>120</v>
       </c>
@@ -8179,7 +8489,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="31.5" hidden="1" thickBot="1">
+    <row r="40" spans="1:16" ht="31.5" thickBot="1">
       <c r="A40" s="6" t="s">
         <v>120</v>
       </c>
@@ -16744,11 +17054,7 @@
       <c r="F404" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I404" xr:uid="{23FEA767-FEF3-4D23-9143-13AEAC680DA5}">
-    <filterColumn colId="7">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I404" xr:uid="{23FEA767-FEF3-4D23-9143-13AEAC680DA5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16757,7 +17063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7DD0CD-6695-4D3C-9518-BDB565BCCF21}">
   <dimension ref="B3:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -16781,129 +17087,268 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FAF9D8E-5017-468F-8689-A64B44F82814}">
-  <dimension ref="E5:F28"/>
+  <dimension ref="B2:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="85.140625" customWidth="1"/>
+    <col min="2" max="2" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="178.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:6">
-      <c r="E5" s="16" t="s">
+    <row r="2" spans="2:3">
+      <c r="B2" s="16" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="6" spans="5:6" ht="201" customHeight="1">
-      <c r="E6" s="16" t="s">
+    <row r="3" spans="2:3" ht="201" customHeight="1">
+      <c r="B3" s="16" t="s">
         <v>813</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="7" spans="5:6">
-      <c r="E7" s="16" t="s">
+    <row r="4" spans="2:3">
+      <c r="B4" s="16" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="8" spans="5:6">
-      <c r="E8" s="16" t="s">
+    <row r="5" spans="2:3">
+      <c r="B5" s="16" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="9" spans="5:6">
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" spans="5:6">
-      <c r="E10" s="16" t="s">
+    <row r="6" spans="2:3">
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="16" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="11" spans="5:6">
-      <c r="E11" s="16" t="s">
+    <row r="8" spans="2:3">
+      <c r="B8" s="16" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="12" spans="5:6">
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="5:6">
-      <c r="E13" s="16" t="s">
+    <row r="9" spans="2:3">
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="16" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="14" spans="5:6">
-      <c r="E14" s="16" t="s">
+    <row r="11" spans="2:3">
+      <c r="B11" s="16" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="15" spans="5:6">
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="5:6">
-      <c r="E16" s="16" t="s">
+    <row r="12" spans="2:3">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="16" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="17" spans="5:5">
-      <c r="E17" s="16" t="s">
+    <row r="14" spans="2:3">
+      <c r="B14" s="16" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="18" spans="5:5">
-      <c r="E18" s="16" t="s">
+    <row r="15" spans="2:3">
+      <c r="B15" s="16" t="s">
         <v>822</v>
       </c>
     </row>
-    <row r="19" spans="5:5">
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="5:5">
-      <c r="E20" s="16" t="s">
+    <row r="16" spans="2:3">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="16" t="s">
         <v>823</v>
       </c>
     </row>
-    <row r="21" spans="5:5">
-      <c r="E21" s="16" t="s">
+    <row r="18" spans="2:4">
+      <c r="B18" s="16" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="22" spans="5:5">
-      <c r="E22" s="16" t="s">
+    <row r="19" spans="2:4">
+      <c r="B19" s="16" t="s">
         <v>825</v>
       </c>
     </row>
-    <row r="23" spans="5:5">
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="5:5">
-      <c r="E24" s="16" t="s">
+    <row r="20" spans="2:4">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="16" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="25" spans="5:5">
-      <c r="E25" s="16" t="s">
+    <row r="22" spans="2:4">
+      <c r="B22" s="16" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="26" spans="5:5">
-      <c r="E26" s="16" t="s">
+    <row r="23" spans="2:4">
+      <c r="B23" s="16" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="27" spans="5:5">
-      <c r="E27" s="16" t="s">
+    <row r="24" spans="2:4">
+      <c r="B24" s="16" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="28" spans="5:5">
-      <c r="E28" s="16" t="s">
+    <row r="25" spans="2:4">
+      <c r="B25" s="16" t="s">
         <v>830</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B28" s="18" t="s">
+        <v>832</v>
+      </c>
+      <c r="C28" s="19"/>
+    </row>
+    <row r="29" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B29" s="18" t="s">
+        <v>833</v>
+      </c>
+      <c r="C29" s="19"/>
+    </row>
+    <row r="30" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B30" s="18" t="s">
+        <v>834</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="2" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B31" s="18" t="s">
+        <v>835</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="2" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B32" s="18" t="s">
+        <v>836</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="2" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B33" s="18" t="s">
+        <v>837</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="2" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B34" s="18" t="s">
+        <v>838</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="2" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B35" s="18" t="s">
+        <v>839</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="2" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B36" s="18" t="s">
+        <v>840</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="2" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B37" s="18" t="s">
+        <v>841</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="2" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B38" s="18" t="s">
+        <v>842</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="2" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B39" s="18" t="s">
+        <v>843</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="2" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B40" s="18" t="s">
+        <v>844</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="2" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B41" s="18" t="s">
+        <v>845</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="2" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B42" s="18" t="s">
+        <v>846</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="2" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="44.25" customHeight="1">
+      <c r="B43" s="18" t="s">
+        <v>847</v>
+      </c>
+      <c r="C43" s="19"/>
+      <c r="D43" s="2" t="s">
+        <v>859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implement procurement lead-time suites and related domain updates
</commit_message>
<xml_diff>
--- a/tests/C2Pro_Test_Suites_Master.xlsx
+++ b/tests/C2Pro_Test_Suites_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esus_\Documents\AI\ZTWQ\c2pro\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E2ED11-DD88-49A3-AD97-0E4F17FD7B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638CA2D0-AAC5-4415-BD7E-DD67DB7B7266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3608" uniqueCount="863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3742" uniqueCount="863">
   <si>
     <t>Nº</t>
   </si>
@@ -3383,7 +3383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3440,9 +3440,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -3754,7 +3751,7 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
@@ -6969,7 +6966,7 @@
       <c r="A103" t="s">
         <v>107</v>
       </c>
-      <c r="B103" s="22" t="s">
+      <c r="B103" s="21" t="s">
         <v>220</v>
       </c>
       <c r="C103" t="s">
@@ -7404,8 +7401,8 @@
   <dimension ref="A1:Q404"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J198" sqref="J198"/>
+      <pane ySplit="1" topLeftCell="A319" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A332" sqref="A332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -13344,6 +13341,9 @@
       <c r="H199" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J199" t="s">
+        <v>404</v>
+      </c>
       <c r="K199" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_002_r6_deviation_5_percent_pass</v>
@@ -13370,6 +13370,9 @@
       <c r="H200" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J200" t="s">
+        <v>404</v>
+      </c>
       <c r="K200" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_003_r6_deviation_4_9_percent_pass</v>
@@ -13396,6 +13399,9 @@
       <c r="H201" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J201" t="s">
+        <v>404</v>
+      </c>
       <c r="K201" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_004_r6_over_budget_critical</v>
@@ -13422,6 +13428,9 @@
       <c r="H202" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J202" t="s">
+        <v>404</v>
+      </c>
       <c r="K202" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_005_r6_under_budget_warning</v>
@@ -13448,6 +13457,9 @@
       <c r="H203" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J203" t="s">
+        <v>404</v>
+      </c>
       <c r="K203" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_006_r6_exact_match_pass</v>
@@ -13474,6 +13486,9 @@
       <c r="H204" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J204" t="s">
+        <v>404</v>
+      </c>
       <c r="K204" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_007_r15_bom_no_budget_alert</v>
@@ -13500,6 +13515,9 @@
       <c r="H205" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J205" t="s">
+        <v>404</v>
+      </c>
       <c r="K205" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_008_r15_bom_with_budget_pass</v>
@@ -13526,6 +13544,9 @@
       <c r="H206" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J206" t="s">
+        <v>404</v>
+      </c>
       <c r="K206" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_009_r15_bom_client_provided_exception</v>
@@ -13552,6 +13573,9 @@
       <c r="H207" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J207" t="s">
+        <v>404</v>
+      </c>
       <c r="K207" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_010_r15_multiple_bom_violations</v>
@@ -13578,6 +13602,9 @@
       <c r="H208" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J208" t="s">
+        <v>404</v>
+      </c>
       <c r="K208" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_011_r15_affected_items_list</v>
@@ -13604,6 +13631,9 @@
       <c r="H209" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J209" t="s">
+        <v>404</v>
+      </c>
       <c r="K209" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_012_r16_deviation_11_percent_alert</v>
@@ -13630,6 +13660,9 @@
       <c r="H210" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J210" t="s">
+        <v>404</v>
+      </c>
       <c r="K210" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_013_r16_deviation_10_percent_pass</v>
@@ -13656,6 +13689,9 @@
       <c r="H211" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J211" t="s">
+        <v>404</v>
+      </c>
       <c r="K211" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_014_r16_over_budget_critical</v>
@@ -13682,6 +13718,9 @@
       <c r="H212" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J212" t="s">
+        <v>404</v>
+      </c>
       <c r="K212" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_015_r16_under_budget_different_severity</v>
@@ -13708,6 +13747,9 @@
       <c r="H213" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J213" t="s">
+        <v>404</v>
+      </c>
       <c r="K213" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-002test_016_r16_trend_calculation</v>
@@ -13737,6 +13779,9 @@
       <c r="I214" t="s">
         <v>809</v>
       </c>
+      <c r="J214" t="s">
+        <v>404</v>
+      </c>
       <c r="K214" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-003test_001_r1_dates_mismatch_alert</v>
@@ -13763,6 +13808,9 @@
       <c r="H215" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J215" t="s">
+        <v>404</v>
+      </c>
       <c r="K215" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-003test_002_r1_dates_match_pass</v>
@@ -13789,6 +13837,9 @@
       <c r="H216" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J216" t="s">
+        <v>404</v>
+      </c>
       <c r="K216" t="str">
         <f t="shared" si="2"/>
         <v>TS-UD-COH-RUL-003test_003_r1_schedule_late_critical</v>
@@ -13815,6 +13866,9 @@
       <c r="H217" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J217" t="s">
+        <v>404</v>
+      </c>
       <c r="K217" t="str">
         <f t="shared" ref="K217:K280" si="3">CONCATENATE(A217,C217)</f>
         <v>TS-UD-COH-RUL-003test_004_r1_schedule_early_warning</v>
@@ -13841,6 +13895,9 @@
       <c r="H218" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J218" t="s">
+        <v>404</v>
+      </c>
       <c r="K218" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_005_r1_delta_days_calculation</v>
@@ -13867,6 +13924,9 @@
       <c r="H219" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J219" t="s">
+        <v>404</v>
+      </c>
       <c r="K219" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_006_r2_milestone_no_activity_alert</v>
@@ -13893,6 +13953,9 @@
       <c r="H220" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J220" t="s">
+        <v>404</v>
+      </c>
       <c r="K220" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_007_r2_milestone_with_activity_pass</v>
@@ -13919,6 +13982,9 @@
       <c r="H221" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J221" t="s">
+        <v>404</v>
+      </c>
       <c r="K221" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_008_r2_milestone_date_mismatch_alert</v>
@@ -13945,6 +14011,9 @@
       <c r="H222" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J222" t="s">
+        <v>404</v>
+      </c>
       <c r="K222" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_009_r2_multiple_milestones_violations</v>
@@ -13971,6 +14040,9 @@
       <c r="H223" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J223" t="s">
+        <v>404</v>
+      </c>
       <c r="K223" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_010_r2_unlinked_milestones_list</v>
@@ -13997,6 +14069,9 @@
       <c r="H224" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J224" t="s">
+        <v>404</v>
+      </c>
       <c r="K224" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_011_r5_activity_exceeds_contract_alert</v>
@@ -14023,6 +14098,9 @@
       <c r="H225" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J225" t="s">
+        <v>404</v>
+      </c>
       <c r="K225" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_012_r5_activity_within_contract_pass</v>
@@ -14049,6 +14127,9 @@
       <c r="H226" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J226" t="s">
+        <v>404</v>
+      </c>
       <c r="K226" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_013_r5_exceeding_activities_list</v>
@@ -14075,6 +14156,9 @@
       <c r="H227" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J227" t="s">
+        <v>404</v>
+      </c>
       <c r="K227" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_014_r5_alert_severity_critical</v>
@@ -14101,6 +14185,9 @@
       <c r="H228" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J228" t="s">
+        <v>404</v>
+      </c>
       <c r="K228" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_015_r14_order_date_passed_critical</v>
@@ -14127,6 +14214,9 @@
       <c r="H229" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J229" t="s">
+        <v>404</v>
+      </c>
       <c r="K229" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-003test_016_r14_order_date_tight_warning</v>
@@ -14145,6 +14235,9 @@
       <c r="D230" s="6"/>
       <c r="E230" s="7"/>
       <c r="F230" s="5"/>
+      <c r="J230" t="s">
+        <v>404</v>
+      </c>
       <c r="K230" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-004Tests not individually listed</v>
@@ -14163,6 +14256,9 @@
       <c r="D231" s="6"/>
       <c r="E231" s="7"/>
       <c r="F231" s="5"/>
+      <c r="J231" t="s">
+        <v>404</v>
+      </c>
       <c r="K231" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-005Tests not individually listed</v>
@@ -14181,6 +14277,9 @@
       <c r="D232" s="6"/>
       <c r="E232" s="7"/>
       <c r="F232" s="5"/>
+      <c r="J232" t="s">
+        <v>404</v>
+      </c>
       <c r="K232" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-RUL-006Tests not individually listed</v>
@@ -14210,7 +14309,9 @@
       <c r="I233" s="12" t="s">
         <v>809</v>
       </c>
-      <c r="J233" s="21"/>
+      <c r="J233" t="s">
+        <v>404</v>
+      </c>
       <c r="K233" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_001_subscore_no_alerts_100_percent</v>
@@ -14237,6 +14338,9 @@
       <c r="H234" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J234" t="s">
+        <v>404</v>
+      </c>
       <c r="K234" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_002_subscore_one_alert_penalized</v>
@@ -14263,6 +14367,9 @@
       <c r="H235" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J235" t="s">
+        <v>404</v>
+      </c>
       <c r="K235" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_003_subscore_multiple_alerts_cumulative</v>
@@ -14289,6 +14396,9 @@
       <c r="H236" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J236" t="s">
+        <v>404</v>
+      </c>
       <c r="K236" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_004_subscore_severity_low_penalty_5</v>
@@ -14315,6 +14425,9 @@
       <c r="H237" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J237" t="s">
+        <v>404</v>
+      </c>
       <c r="K237" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_005_subscore_severity_medium_penalty_10</v>
@@ -14341,6 +14454,9 @@
       <c r="H238" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J238" t="s">
+        <v>404</v>
+      </c>
       <c r="K238" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_006_subscore_severity_high_penalty_20</v>
@@ -14367,6 +14483,9 @@
       <c r="H239" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J239" t="s">
+        <v>404</v>
+      </c>
       <c r="K239" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_007_subscore_severity_critical_penalty_30</v>
@@ -14393,6 +14512,9 @@
       <c r="H240" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J240" t="s">
+        <v>404</v>
+      </c>
       <c r="K240" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_008_subscore_scope_calculation</v>
@@ -14419,6 +14541,9 @@
       <c r="H241" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J241" t="s">
+        <v>404</v>
+      </c>
       <c r="K241" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_009_subscore_budget_calculation</v>
@@ -14445,6 +14570,9 @@
       <c r="H242" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J242" t="s">
+        <v>404</v>
+      </c>
       <c r="K242" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_010_subscore_quality_calculation</v>
@@ -14471,6 +14599,9 @@
       <c r="H243" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J243" t="s">
+        <v>404</v>
+      </c>
       <c r="K243" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_011_subscore_technical_calculation</v>
@@ -14497,6 +14628,9 @@
       <c r="H244" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J244" t="s">
+        <v>404</v>
+      </c>
       <c r="K244" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_012_subscore_legal_calculation</v>
@@ -14523,6 +14657,9 @@
       <c r="H245" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J245" t="s">
+        <v>404</v>
+      </c>
       <c r="K245" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_013_subscore_time_calculation</v>
@@ -14549,6 +14686,9 @@
       <c r="H246" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J246" t="s">
+        <v>404</v>
+      </c>
       <c r="K246" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-001test_014_subscore_floor_at_zero</v>
@@ -14575,6 +14715,9 @@
       <c r="H247" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J247" t="s">
+        <v>404</v>
+      </c>
       <c r="K247" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_001_global_score_formula_verification</v>
@@ -14601,6 +14744,9 @@
       <c r="H248" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J248" t="s">
+        <v>404</v>
+      </c>
       <c r="K248" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_002_global_score_default_weights</v>
@@ -14627,6 +14773,9 @@
       <c r="H249" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J249" t="s">
+        <v>404</v>
+      </c>
       <c r="K249" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_003_global_score_all_100_equals_100</v>
@@ -14653,6 +14802,9 @@
       <c r="H250" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J250" t="s">
+        <v>404</v>
+      </c>
       <c r="K250" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_004_global_score_all_0_equals_0</v>
@@ -14679,6 +14831,9 @@
       <c r="H251" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J251" t="s">
+        <v>404</v>
+      </c>
       <c r="K251" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_005_global_score_mixed_subscores</v>
@@ -14705,6 +14860,9 @@
       <c r="H252" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J252" t="s">
+        <v>404</v>
+      </c>
       <c r="K252" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_006_global_score_range_0_to_100</v>
@@ -14731,6 +14889,9 @@
       <c r="H253" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J253" t="s">
+        <v>404</v>
+      </c>
       <c r="K253" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_007_weights_sum_validation</v>
@@ -14757,6 +14918,9 @@
       <c r="H254" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J254" t="s">
+        <v>404</v>
+      </c>
       <c r="K254" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_008_weights_normalization_auto</v>
@@ -14783,6 +14947,9 @@
       <c r="H255" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J255" t="s">
+        <v>404</v>
+      </c>
       <c r="K255" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_009_weights_custom_budget_30</v>
@@ -14809,6 +14976,9 @@
       <c r="H256" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J256" t="s">
+        <v>404</v>
+      </c>
       <c r="K256" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_010_weights_custom_time_25</v>
@@ -14835,6 +15005,9 @@
       <c r="H257" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J257" t="s">
+        <v>404</v>
+      </c>
       <c r="K257" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_011_weights_per_project_type</v>
@@ -14861,6 +15034,9 @@
       <c r="H258" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J258" t="s">
+        <v>404</v>
+      </c>
       <c r="K258" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-SCR-002test_012_weights_history_tracking</v>
@@ -14879,6 +15055,9 @@
       <c r="D259" s="6"/>
       <c r="E259" s="7"/>
       <c r="F259" s="5"/>
+      <c r="J259" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="260" spans="1:11" ht="31.5" thickBot="1">
       <c r="A260" s="6" t="s">
@@ -14901,6 +15080,9 @@
       <c r="H260" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J260" t="s">
+        <v>404</v>
+      </c>
       <c r="K260" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_001_detect_mass_changes_15_in_30min</v>
@@ -14927,6 +15109,9 @@
       <c r="H261" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J261" t="s">
+        <v>404</v>
+      </c>
       <c r="K261" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_002_no_violation_10_in_60min</v>
@@ -14953,6 +15138,9 @@
       <c r="H262" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J262" t="s">
+        <v>404</v>
+      </c>
       <c r="K262" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_003_mass_changes_window_sliding</v>
@@ -14979,6 +15167,9 @@
       <c r="H263" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J263" t="s">
+        <v>404</v>
+      </c>
       <c r="K263" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_004_mass_changes_flag_for_review</v>
@@ -15005,6 +15196,9 @@
       <c r="H264" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J264" t="s">
+        <v>404</v>
+      </c>
       <c r="K264" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_005_detect_resolve_reintroduce_4_times</v>
@@ -15031,6 +15225,9 @@
       <c r="H265" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J265" t="s">
+        <v>404</v>
+      </c>
       <c r="K265" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_006_no_violation_2_times</v>
@@ -15057,6 +15254,9 @@
       <c r="H266" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J266" t="s">
+        <v>404</v>
+      </c>
       <c r="K266" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_007_hash_comparison_same_content</v>
@@ -15083,6 +15283,9 @@
       <c r="H267" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J267" t="s">
+        <v>404</v>
+      </c>
       <c r="K267" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_008_penalty_minus_5_points</v>
@@ -15109,6 +15312,9 @@
       <c r="H268" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J268" t="s">
+        <v>404</v>
+      </c>
       <c r="K268" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_009_detect_95_percent_3_docs</v>
@@ -15135,6 +15341,9 @@
       <c r="H269" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J269" t="s">
+        <v>404</v>
+      </c>
       <c r="K269" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_010_no_violation_95_percent_50_docs</v>
@@ -15161,6 +15370,9 @@
       <c r="H270" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J270" t="s">
+        <v>404</v>
+      </c>
       <c r="K270" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_011_threshold_90_percent_5_docs</v>
@@ -15187,6 +15399,9 @@
       <c r="H271" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J271" t="s">
+        <v>404</v>
+      </c>
       <c r="K271" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_012_require_audit_action</v>
@@ -15213,6 +15428,9 @@
       <c r="H272" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J272" t="s">
+        <v>404</v>
+      </c>
       <c r="K272" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_013_detect_weight_change_25_percent</v>
@@ -15239,6 +15457,9 @@
       <c r="H273" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J273" t="s">
+        <v>404</v>
+      </c>
       <c r="K273" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_014_no_violation_change_15_percent</v>
@@ -15265,6 +15486,9 @@
       <c r="H274" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J274" t="s">
+        <v>404</v>
+      </c>
       <c r="K274" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_015_24h_window_tracking</v>
@@ -15291,6 +15515,9 @@
       <c r="H275" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J275" t="s">
+        <v>404</v>
+      </c>
       <c r="K275" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-GAM-001test_016_notify_admin_action</v>
@@ -15309,6 +15536,9 @@
       <c r="D276" s="6"/>
       <c r="E276" s="7"/>
       <c r="F276" s="5"/>
+      <c r="J276" t="s">
+        <v>404</v>
+      </c>
       <c r="K276" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-COH-ALR-001Tests not individually listed</v>
@@ -15338,6 +15568,9 @@
       <c r="I277" t="s">
         <v>810</v>
       </c>
+      <c r="J277" t="s">
+        <v>404</v>
+      </c>
       <c r="K277" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-PRJ-WBS-001test_001_wbs_item_creation_all_fields</v>
@@ -15364,6 +15597,9 @@
       <c r="H278" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J278" t="s">
+        <v>404</v>
+      </c>
       <c r="K278" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-PRJ-WBS-001test_002_wbs_item_creation_minimum_fields</v>
@@ -15390,6 +15626,9 @@
       <c r="H279" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J279" t="s">
+        <v>404</v>
+      </c>
       <c r="K279" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-PRJ-WBS-001test_003_wbs_item_fails_without_code</v>
@@ -15416,6 +15655,9 @@
       <c r="H280" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J280" t="s">
+        <v>404</v>
+      </c>
       <c r="K280" t="str">
         <f t="shared" si="3"/>
         <v>TS-UD-PRJ-WBS-001test_004_wbs_item_fails_without_name</v>
@@ -15442,6 +15684,9 @@
       <c r="H281" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J281" t="s">
+        <v>404</v>
+      </c>
       <c r="K281" t="str">
         <f t="shared" ref="K281:K331" si="4">CONCATENATE(A281,C281)</f>
         <v>TS-UD-PRJ-WBS-001test_005_wbs_item_fails_invalid_level</v>
@@ -15468,6 +15713,9 @@
       <c r="H282" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J282" t="s">
+        <v>404</v>
+      </c>
       <c r="K282" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_006_wbs_item_immutability</v>
@@ -15494,6 +15742,9 @@
       <c r="H283" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J283" t="s">
+        <v>404</v>
+      </c>
       <c r="K283" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_007_wbs_code_format_1</v>
@@ -15520,6 +15771,9 @@
       <c r="H284" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J284" t="s">
+        <v>404</v>
+      </c>
       <c r="K284" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_008_wbs_code_format_1_1</v>
@@ -15546,6 +15800,9 @@
       <c r="H285" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J285" t="s">
+        <v>404</v>
+      </c>
       <c r="K285" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_009_wbs_code_format_1_1_1</v>
@@ -15572,6 +15829,9 @@
       <c r="H286" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J286" t="s">
+        <v>404</v>
+      </c>
       <c r="K286" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_010_wbs_code_format_1_1_1_1</v>
@@ -15598,6 +15858,9 @@
       <c r="H287" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J287" t="s">
+        <v>404</v>
+      </c>
       <c r="K287" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_011_wbs_code_invalid_format_rejected</v>
@@ -15624,6 +15887,9 @@
       <c r="H288" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J288" t="s">
+        <v>404</v>
+      </c>
       <c r="K288" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_012_wbs_code_uniqueness_per_project</v>
@@ -15650,6 +15916,9 @@
       <c r="H289" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J289" t="s">
+        <v>404</v>
+      </c>
       <c r="K289" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_013_wbs_level_1_valid</v>
@@ -15676,6 +15945,9 @@
       <c r="H290" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J290" t="s">
+        <v>404</v>
+      </c>
       <c r="K290" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_014_wbs_level_4_valid</v>
@@ -15702,6 +15974,9 @@
       <c r="H291" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J291" t="s">
+        <v>404</v>
+      </c>
       <c r="K291" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_015_wbs_level_0_invalid</v>
@@ -15728,6 +16003,9 @@
       <c r="H292" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J292" t="s">
+        <v>404</v>
+      </c>
       <c r="K292" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_016_wbs_level_5_invalid</v>
@@ -15754,6 +16032,9 @@
       <c r="H293" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J293" t="s">
+        <v>404</v>
+      </c>
       <c r="K293" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_017_wbs_level_matches_code_depth</v>
@@ -15780,6 +16061,9 @@
       <c r="H294" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J294" t="s">
+        <v>404</v>
+      </c>
       <c r="K294" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-001test_018_wbs_level_parent_child_validation</v>
@@ -15798,6 +16082,9 @@
       <c r="D295" s="6"/>
       <c r="E295" s="7"/>
       <c r="F295" s="5"/>
+      <c r="J295" t="s">
+        <v>404</v>
+      </c>
       <c r="K295" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-002Tests not individually listed</v>
@@ -15816,6 +16103,9 @@
       <c r="D296" s="6"/>
       <c r="E296" s="7"/>
       <c r="F296" s="5"/>
+      <c r="J296" t="s">
+        <v>404</v>
+      </c>
       <c r="K296" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-003Tests not individually listed</v>
@@ -15834,6 +16124,9 @@
       <c r="D297" s="6"/>
       <c r="E297" s="7"/>
       <c r="F297" s="5"/>
+      <c r="J297" t="s">
+        <v>404</v>
+      </c>
       <c r="K297" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-WBS-004Tests not individually listed</v>
@@ -15852,6 +16145,9 @@
       <c r="D298" s="6"/>
       <c r="E298" s="7"/>
       <c r="F298" s="5"/>
+      <c r="J298" t="s">
+        <v>404</v>
+      </c>
       <c r="K298" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-PRJ-001Tests not individually listed</v>
@@ -15870,6 +16166,9 @@
       <c r="D299" s="6"/>
       <c r="E299" s="7"/>
       <c r="F299" s="5"/>
+      <c r="J299" t="s">
+        <v>404</v>
+      </c>
       <c r="K299" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PRJ-DTO-001Tests not individually listed</v>
@@ -15888,6 +16187,9 @@
       <c r="D300" s="6"/>
       <c r="E300" s="7"/>
       <c r="F300" s="5"/>
+      <c r="J300" t="s">
+        <v>404</v>
+      </c>
       <c r="K300" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-BOM-001Tests not individually listed</v>
@@ -15906,6 +16208,9 @@
       <c r="D301" s="6"/>
       <c r="E301" s="7"/>
       <c r="F301" s="5"/>
+      <c r="J301" t="s">
+        <v>404</v>
+      </c>
       <c r="K301" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-BOM-002Tests not individually listed</v>
@@ -15935,6 +16240,9 @@
       <c r="I302" t="s">
         <v>811</v>
       </c>
+      <c r="J302" t="s">
+        <v>404</v>
+      </c>
       <c r="K302" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_001_optimal_date_production_only</v>
@@ -15961,6 +16269,9 @@
       <c r="H303" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J303" t="s">
+        <v>404</v>
+      </c>
       <c r="K303" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_002_optimal_date_production_transit</v>
@@ -15987,6 +16298,9 @@
       <c r="H304" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J304" t="s">
+        <v>404</v>
+      </c>
       <c r="K304" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_003_optimal_date_production_transit_buffer</v>
@@ -16013,6 +16327,9 @@
       <c r="H305" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J305" t="s">
+        <v>404</v>
+      </c>
       <c r="K305" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_004_optimal_date_all_components</v>
@@ -16039,6 +16356,9 @@
       <c r="H306" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J306" t="s">
+        <v>404</v>
+      </c>
       <c r="K306" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_005_lead_time_breakdown_returned</v>
@@ -16065,6 +16385,9 @@
       <c r="H307" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J307" t="s">
+        <v>404</v>
+      </c>
       <c r="K307" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_006_required_on_site_calculation</v>
@@ -16091,6 +16414,9 @@
       <c r="H308" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J308" t="s">
+        <v>404</v>
+      </c>
       <c r="K308" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_007_business_days_calculation</v>
@@ -16117,6 +16443,9 @@
       <c r="H309" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J309" t="s">
+        <v>404</v>
+      </c>
       <c r="K309" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_008_weekend_exclusion</v>
@@ -16143,6 +16472,9 @@
       <c r="H310" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J310" t="s">
+        <v>404</v>
+      </c>
       <c r="K310" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_009_holiday_exclusion</v>
@@ -16169,6 +16501,9 @@
       <c r="H311" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J311" t="s">
+        <v>404</v>
+      </c>
       <c r="K311" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_010_delivery_on_weekend_adjusted</v>
@@ -16195,6 +16530,9 @@
       <c r="H312" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J312" t="s">
+        <v>404</v>
+      </c>
       <c r="K312" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_011_mixed_calendar_business_days</v>
@@ -16221,6 +16559,9 @@
       <c r="H313" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J313" t="s">
+        <v>404</v>
+      </c>
       <c r="K313" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_012_alert_r14_date_passed</v>
@@ -16247,6 +16588,9 @@
       <c r="H314" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J314" t="s">
+        <v>404</v>
+      </c>
       <c r="K314" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_013_alert_r14_tight_margin_3_days</v>
@@ -16273,6 +16617,9 @@
       <c r="H315" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J315" t="s">
+        <v>404</v>
+      </c>
       <c r="K315" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_014_alert_severity_critical_passed</v>
@@ -16299,6 +16646,9 @@
       <c r="H316" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J316" t="s">
+        <v>404</v>
+      </c>
       <c r="K316" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_015_alert_severity_warning_tight</v>
@@ -16325,6 +16675,9 @@
       <c r="H317" s="12" t="s">
         <v>407</v>
       </c>
+      <c r="J317" t="s">
+        <v>404</v>
+      </c>
       <c r="K317" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-001test_016_no_alert_sufficient_margin</v>
@@ -16348,6 +16701,9 @@
       <c r="G318" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J318" t="s">
+        <v>404</v>
+      </c>
       <c r="K318" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_001_exw_buyer_full_responsibility</v>
@@ -16371,6 +16727,9 @@
       <c r="G319" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J319" t="s">
+        <v>404</v>
+      </c>
       <c r="K319" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_002_exw_transit_time_included</v>
@@ -16394,6 +16753,9 @@
       <c r="G320" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J320" t="s">
+        <v>404</v>
+      </c>
       <c r="K320" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_003_exw_customs_included</v>
@@ -16417,6 +16779,9 @@
       <c r="G321" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J321" t="s">
+        <v>404</v>
+      </c>
       <c r="K321" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_004_fob_shared_responsibility</v>
@@ -16440,6 +16805,9 @@
       <c r="G322" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J322" t="s">
+        <v>404</v>
+      </c>
       <c r="K322" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_005_fob_port_handover</v>
@@ -16463,6 +16831,9 @@
       <c r="G323" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J323" t="s">
+        <v>404</v>
+      </c>
       <c r="K323" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_006_fob_insurance_buyer</v>
@@ -16486,6 +16857,9 @@
       <c r="G324" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J324" t="s">
+        <v>404</v>
+      </c>
       <c r="K324" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_007_cif_seller_insurance</v>
@@ -16509,6 +16883,9 @@
       <c r="G325" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J325" t="s">
+        <v>404</v>
+      </c>
       <c r="K325" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_008_cif_port_to_port</v>
@@ -16532,6 +16909,9 @@
       <c r="G326" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J326" t="s">
+        <v>404</v>
+      </c>
       <c r="K326" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_009_cif_customs_buyer</v>
@@ -16555,6 +16935,9 @@
       <c r="G327" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J327" t="s">
+        <v>404</v>
+      </c>
       <c r="K327" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_010_ddp_seller_full_responsibility</v>
@@ -16578,6 +16961,9 @@
       <c r="G328" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J328" t="s">
+        <v>404</v>
+      </c>
       <c r="K328" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_011_ddp_no_customs_buyer</v>
@@ -16601,6 +16987,9 @@
       <c r="G329" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J329" t="s">
+        <v>404</v>
+      </c>
       <c r="K329" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_012_ddp_door_to_door</v>
@@ -16624,6 +17013,9 @@
       <c r="G330" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J330" t="s">
+        <v>404</v>
+      </c>
       <c r="K330" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_013_incoterm_comparison_same_route</v>
@@ -16647,6 +17039,9 @@
       <c r="G331" s="12" t="s">
         <v>771</v>
       </c>
+      <c r="J331" t="s">
+        <v>404</v>
+      </c>
       <c r="K331" t="str">
         <f t="shared" si="4"/>
         <v>TS-UD-PROC-LTM-002test_014_incoterm_impact_on_lead_time</v>
@@ -16665,6 +17060,9 @@
       <c r="D332" s="6"/>
       <c r="E332" s="7"/>
       <c r="F332" s="5"/>
+      <c r="J332" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="333" spans="1:11" ht="16.5" thickBot="1">
       <c r="A333" s="6" t="s">
@@ -17672,7 +18070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7DD0CD-6695-4D3C-9518-BDB565BCCF21}">
   <dimension ref="B3:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chore: update tests and adapters
</commit_message>
<xml_diff>
--- a/tests/C2Pro_Test_Suites_Master.xlsx
+++ b/tests/C2Pro_Test_Suites_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esus_\Documents\AI\ZTWQ\c2pro\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79CD580-3D6E-41EC-ADBC-0888C41D8202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887C8B13-CE69-4AF6-9C3E-FBB8B4CF3DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20616" windowHeight="11016" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suite Test" sheetId="1" r:id="rId1"/>
@@ -3930,9 +3930,6 @@
     <t>AGENTE</t>
   </si>
   <si>
-    <t>orden</t>
-  </si>
-  <si>
     <t>7- skateholders</t>
   </si>
   <si>
@@ -3985,6 +3982,9 @@
   </si>
   <si>
     <t>14 - QA/E2E</t>
+  </si>
+  <si>
+    <t>prioridad</t>
   </si>
 </sst>
 </file>
@@ -4593,8 +4593,8 @@
   <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="19.2" customHeight="1"/>
@@ -8712,9 +8712,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FEA767-FEF3-4D23-9143-13AEAC680DA5}">
   <dimension ref="A1:Q404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A330" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F338" sqref="F338:F402"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -8725,8 +8725,9 @@
     <col min="4" max="4" width="11.5546875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="50.5546875" customWidth="1"/>
-    <col min="7" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="10" width="39.5546875" customWidth="1"/>
+    <col min="7" max="8" width="11.5546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="39.5546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="39.5546875" customWidth="1"/>
     <col min="11" max="11" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -18474,7 +18475,7 @@
       <c r="D338" s="6"/>
       <c r="E338" s="7"/>
       <c r="F338" s="5" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="339" spans="1:10" ht="16.2" thickBot="1">
@@ -18490,7 +18491,7 @@
       <c r="D339" s="6"/>
       <c r="E339" s="7"/>
       <c r="F339" s="5" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="340" spans="1:10" ht="16.2" thickBot="1">
@@ -18506,7 +18507,7 @@
       <c r="D340" s="6"/>
       <c r="E340" s="7"/>
       <c r="F340" s="5" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="341" spans="1:10" ht="16.2" thickBot="1">
@@ -18522,7 +18523,7 @@
       <c r="D341" s="6"/>
       <c r="E341" s="7"/>
       <c r="F341" s="5" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="342" spans="1:10" ht="16.2" thickBot="1">
@@ -18538,7 +18539,7 @@
       <c r="D342" s="6"/>
       <c r="E342" s="7"/>
       <c r="F342" s="5" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="343" spans="1:10" ht="16.2" thickBot="1">
@@ -18554,7 +18555,7 @@
       <c r="D343" s="6"/>
       <c r="E343" s="7"/>
       <c r="F343" s="5" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="344" spans="1:10" ht="16.2" thickBot="1">
@@ -18570,7 +18571,7 @@
       <c r="D344" s="6"/>
       <c r="E344" s="7"/>
       <c r="F344" s="5" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="345" spans="1:10" ht="16.2" thickBot="1">
@@ -18586,7 +18587,7 @@
       <c r="D345" s="6"/>
       <c r="E345" s="7"/>
       <c r="F345" s="5" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="346" spans="1:10" ht="16.2" thickBot="1">
@@ -18602,7 +18603,7 @@
       <c r="D346" s="6"/>
       <c r="E346" s="7"/>
       <c r="F346" s="5" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="347" spans="1:10" ht="16.2" thickBot="1">
@@ -18618,7 +18619,7 @@
       <c r="D347" s="6"/>
       <c r="E347" s="7"/>
       <c r="F347" s="5" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="348" spans="1:10" ht="16.2" thickBot="1">
@@ -18634,7 +18635,7 @@
       <c r="D348" s="6"/>
       <c r="E348" s="7"/>
       <c r="F348" s="5" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="349" spans="1:10" ht="16.2" thickBot="1">
@@ -18650,7 +18651,7 @@
       <c r="D349" s="6"/>
       <c r="E349" s="7"/>
       <c r="F349" s="5" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="350" spans="1:10" ht="16.2" thickBot="1">
@@ -18666,7 +18667,7 @@
       <c r="D350" s="6"/>
       <c r="E350" s="7"/>
       <c r="F350" s="5" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="351" spans="1:10" ht="16.2" thickBot="1">
@@ -18682,7 +18683,7 @@
       <c r="D351" s="6"/>
       <c r="E351" s="7"/>
       <c r="F351" s="5" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="352" spans="1:10" ht="16.2" thickBot="1">
@@ -18698,7 +18699,7 @@
       <c r="D352" s="31"/>
       <c r="E352" s="32"/>
       <c r="F352" s="5" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="J352" t="s">
         <v>404</v>
@@ -18717,7 +18718,7 @@
       <c r="D353" s="31"/>
       <c r="E353" s="32"/>
       <c r="F353" s="5" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="J353" t="s">
         <v>404</v>
@@ -18736,7 +18737,7 @@
       <c r="D354" s="6"/>
       <c r="E354" s="7"/>
       <c r="F354" s="5" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="355" spans="1:10" ht="16.2" thickBot="1">
@@ -18752,7 +18753,7 @@
       <c r="D355" s="6"/>
       <c r="E355" s="7"/>
       <c r="F355" s="5" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="356" spans="1:10" ht="16.2" thickBot="1">
@@ -18768,7 +18769,7 @@
       <c r="D356" s="6"/>
       <c r="E356" s="7"/>
       <c r="F356" s="5" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="357" spans="1:10" ht="16.2" thickBot="1">
@@ -18784,7 +18785,7 @@
       <c r="D357" s="6"/>
       <c r="E357" s="7"/>
       <c r="F357" s="5" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="358" spans="1:10" ht="16.2" thickBot="1">
@@ -18800,7 +18801,7 @@
       <c r="D358" s="6"/>
       <c r="E358" s="7"/>
       <c r="F358" s="5" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="359" spans="1:10" ht="16.2" thickBot="1">
@@ -18816,7 +18817,7 @@
       <c r="D359" s="6"/>
       <c r="E359" s="7"/>
       <c r="F359" s="5" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="360" spans="1:10" ht="16.2" thickBot="1">
@@ -18832,7 +18833,7 @@
       <c r="D360" s="6"/>
       <c r="E360" s="7"/>
       <c r="F360" s="5" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="361" spans="1:10" ht="16.2" thickBot="1">
@@ -18848,7 +18849,7 @@
       <c r="D361" s="6"/>
       <c r="E361" s="7"/>
       <c r="F361" s="5" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="362" spans="1:10" ht="16.2" thickBot="1">
@@ -18864,7 +18865,7 @@
       <c r="D362" s="6"/>
       <c r="E362" s="7"/>
       <c r="F362" s="5" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="363" spans="1:10" ht="16.2" thickBot="1">
@@ -18880,7 +18881,7 @@
       <c r="D363" s="6"/>
       <c r="E363" s="7"/>
       <c r="F363" s="5" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="364" spans="1:10" ht="16.2" thickBot="1">
@@ -18896,7 +18897,7 @@
       <c r="D364" s="6"/>
       <c r="E364" s="7"/>
       <c r="F364" s="5" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="365" spans="1:10" ht="16.2" thickBot="1">
@@ -18912,7 +18913,7 @@
       <c r="D365" s="6"/>
       <c r="E365" s="7"/>
       <c r="F365" s="5" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="366" spans="1:10" ht="16.2" thickBot="1">
@@ -18928,7 +18929,7 @@
       <c r="D366" s="6"/>
       <c r="E366" s="7"/>
       <c r="F366" s="5" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="367" spans="1:10" ht="16.2" thickBot="1">
@@ -18944,7 +18945,7 @@
       <c r="D367" s="6"/>
       <c r="E367" s="7"/>
       <c r="F367" s="5" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="368" spans="1:10" ht="16.2" thickBot="1">
@@ -18960,7 +18961,7 @@
       <c r="D368" s="6"/>
       <c r="E368" s="7"/>
       <c r="F368" s="5" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="369" spans="1:10" ht="16.2" thickBot="1">
@@ -18976,7 +18977,7 @@
       <c r="D369" s="6"/>
       <c r="E369" s="7"/>
       <c r="F369" s="5" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="J369" t="s">
         <v>851</v>
@@ -18995,7 +18996,7 @@
       <c r="D370" s="6"/>
       <c r="E370" s="7"/>
       <c r="F370" s="5" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="J370" t="s">
         <v>851</v>
@@ -19014,7 +19015,7 @@
       <c r="D371" s="6"/>
       <c r="E371" s="7"/>
       <c r="F371" s="5" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="372" spans="1:10" ht="16.2" thickBot="1">
@@ -19030,7 +19031,7 @@
       <c r="D372" s="6"/>
       <c r="E372" s="7"/>
       <c r="F372" s="5" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="373" spans="1:10" ht="16.2" thickBot="1">
@@ -19046,7 +19047,7 @@
       <c r="D373" s="6"/>
       <c r="E373" s="7"/>
       <c r="F373" s="5" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="J373" t="s">
         <v>851</v>
@@ -19065,7 +19066,7 @@
       <c r="D374" s="6"/>
       <c r="E374" s="7"/>
       <c r="F374" s="5" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="375" spans="1:10" ht="16.2" thickBot="1">
@@ -19081,7 +19082,7 @@
       <c r="D375" s="6"/>
       <c r="E375" s="7"/>
       <c r="F375" s="5" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="376" spans="1:10" ht="16.2" thickBot="1">
@@ -19097,7 +19098,7 @@
       <c r="D376" s="6"/>
       <c r="E376" s="7"/>
       <c r="F376" s="5" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="377" spans="1:10" ht="16.2" thickBot="1">
@@ -19113,7 +19114,7 @@
       <c r="D377" s="6"/>
       <c r="E377" s="7"/>
       <c r="F377" s="5" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="378" spans="1:10" ht="16.2" thickBot="1">
@@ -19129,7 +19130,7 @@
       <c r="D378" s="6"/>
       <c r="E378" s="7"/>
       <c r="F378" s="5" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="J378" t="s">
         <v>404</v>
@@ -19148,7 +19149,7 @@
       <c r="D379" s="6"/>
       <c r="E379" s="7"/>
       <c r="F379" s="5" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="J379" t="s">
         <v>404</v>
@@ -19167,7 +19168,7 @@
       <c r="D380" s="6"/>
       <c r="E380" s="7"/>
       <c r="F380" s="5" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="J380" t="s">
         <v>404</v>
@@ -19186,7 +19187,7 @@
       <c r="D381" s="6"/>
       <c r="E381" s="7"/>
       <c r="F381" s="5" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="382" spans="1:10" ht="16.2" thickBot="1">
@@ -19202,7 +19203,7 @@
       <c r="D382" s="6"/>
       <c r="E382" s="7"/>
       <c r="F382" s="5" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="383" spans="1:10" ht="16.2" thickBot="1">
@@ -19218,7 +19219,7 @@
       <c r="D383" s="6"/>
       <c r="E383" s="7"/>
       <c r="F383" s="5" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="384" spans="1:10" ht="16.2" thickBot="1">
@@ -19234,7 +19235,7 @@
       <c r="D384" s="6"/>
       <c r="E384" s="7"/>
       <c r="F384" s="5" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="385" spans="1:10" ht="16.2" thickBot="1">
@@ -19250,7 +19251,7 @@
       <c r="D385" s="6"/>
       <c r="E385" s="7"/>
       <c r="F385" s="5" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="386" spans="1:10" ht="16.2" thickBot="1">
@@ -19266,7 +19267,7 @@
       <c r="D386" s="6"/>
       <c r="E386" s="7"/>
       <c r="F386" s="5" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="387" spans="1:10" ht="16.2" thickBot="1">
@@ -19282,7 +19283,7 @@
       <c r="D387" s="6"/>
       <c r="E387" s="7"/>
       <c r="F387" s="5" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="388" spans="1:10" ht="16.2" thickBot="1">
@@ -19298,7 +19299,7 @@
       <c r="D388" s="6"/>
       <c r="E388" s="7"/>
       <c r="F388" s="5" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="389" spans="1:10" ht="16.2" thickBot="1">
@@ -19314,7 +19315,7 @@
       <c r="D389" s="6"/>
       <c r="E389" s="7"/>
       <c r="F389" s="5" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="390" spans="1:10" ht="16.2" thickBot="1">
@@ -19330,7 +19331,7 @@
       <c r="D390" s="6"/>
       <c r="E390" s="7"/>
       <c r="F390" s="5" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="391" spans="1:10" ht="16.2" thickBot="1">
@@ -19346,7 +19347,7 @@
       <c r="D391" s="6"/>
       <c r="E391" s="7"/>
       <c r="F391" s="5" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="J391" t="s">
         <v>404</v>
@@ -19365,7 +19366,7 @@
       <c r="D392" s="6"/>
       <c r="E392" s="7"/>
       <c r="F392" s="5" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="J392" t="s">
         <v>404</v>
@@ -19384,7 +19385,7 @@
       <c r="D393" s="6"/>
       <c r="E393" s="7"/>
       <c r="F393" s="5" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="J393" t="s">
         <v>404</v>
@@ -19403,7 +19404,7 @@
       <c r="D394" s="6"/>
       <c r="E394" s="7"/>
       <c r="F394" s="5" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="395" spans="1:10" ht="16.2" thickBot="1">
@@ -19419,7 +19420,7 @@
       <c r="D395" s="6"/>
       <c r="E395" s="7"/>
       <c r="F395" s="5" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="396" spans="1:10" ht="16.2" thickBot="1">
@@ -19435,7 +19436,7 @@
       <c r="D396" s="6"/>
       <c r="E396" s="7"/>
       <c r="F396" s="5" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="397" spans="1:10" ht="16.2" thickBot="1">
@@ -19451,7 +19452,7 @@
       <c r="D397" s="21"/>
       <c r="E397" s="30"/>
       <c r="F397" s="5" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="G397" s="20"/>
       <c r="H397" s="20"/>
@@ -19473,7 +19474,7 @@
       <c r="D398" s="6"/>
       <c r="E398" s="7"/>
       <c r="F398" s="5" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="399" spans="1:10" ht="16.2" thickBot="1">
@@ -19489,7 +19490,7 @@
       <c r="D399" s="6"/>
       <c r="E399" s="7"/>
       <c r="F399" s="5" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="400" spans="1:10" ht="16.2" thickBot="1">
@@ -19505,7 +19506,7 @@
       <c r="D400" s="6"/>
       <c r="E400" s="7"/>
       <c r="F400" s="5" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="401" spans="1:6" ht="16.2" thickBot="1">
@@ -19521,7 +19522,7 @@
       <c r="D401" s="6"/>
       <c r="E401" s="7"/>
       <c r="F401" s="5" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="402" spans="1:6" ht="16.2" thickBot="1">
@@ -19537,7 +19538,7 @@
       <c r="D402" s="6"/>
       <c r="E402" s="7"/>
       <c r="F402" s="5" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="403" spans="1:6" ht="15" thickBot="1">
@@ -22471,8 +22472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7AC209-399B-46DE-A186-E777887E2AAF}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -22489,7 +22490,7 @@
         <v>1167</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>1168</v>
+        <v>1186</v>
       </c>
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
@@ -22737,10 +22738,10 @@
       <c r="I15" s="23"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="35" t="s">
         <v>875</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="35" t="s">
         <v>852</v>
       </c>
       <c r="C16" s="29">
@@ -24399,8 +24400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FAF9D8E-5017-468F-8689-A64B44F82814}">
   <dimension ref="A1:J166"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="45" customHeight="1"/>
@@ -25513,7 +25514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7DD0CD-6695-4D3C-9518-BDB565BCCF21}">
   <dimension ref="B3:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chore: commit all remaining workspace changes
</commit_message>
<xml_diff>
--- a/tests/C2Pro_Test_Suites_Master.xlsx
+++ b/tests/C2Pro_Test_Suites_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esus_\Documents\AI\ZTWQ\c2pro\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72E091C-0488-4CD6-A8F3-5226143CCA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6CCB49-8616-4C07-AF9D-87A7743B8679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12480" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5823" uniqueCount="1658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5850" uniqueCount="1660">
   <si>
     <t>Nº</t>
   </si>
@@ -12655,6 +12655,9 @@
   - test_i2_low_confidence_table_routes_to_human_review_conceptually</t>
   </si>
   <si>
+    <t>red</t>
+  </si>
+  <si>
     <t>detectado issue de seguridad</t>
   </si>
   <si>
@@ -12727,7 +12730,10 @@
     <t xml:space="preserve"> @frontend-tdd can then implement GREEN for those new failing tests.</t>
   </si>
   <si>
-    <t xml:space="preserve"> @qa-agent RED plan for S3-0</t>
+    <t>E2E pending</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @qa-agent RED plan for S3-</t>
   </si>
 </sst>
 </file>
@@ -12987,7 +12993,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -13163,6 +13169,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18967,67 +18976,67 @@
     <row r="236" spans="2:2" hidden="1"/>
     <row r="243" spans="1:1">
       <c r="A243" s="16" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" s="16" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" s="16" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" s="16" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" s="16" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" s="16" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" s="16" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" s="16" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" s="16" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" s="16" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" s="16" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" s="16" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" s="16" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
     </row>
   </sheetData>
@@ -39161,8 +39170,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -39545,7 +39554,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="45">
+    <row r="17" spans="1:8" ht="45">
       <c r="A17" s="38" t="s">
         <v>1249</v>
       </c>
@@ -39568,7 +39577,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="60">
+    <row r="18" spans="1:8" ht="60">
       <c r="A18" s="38" t="s">
         <v>1252</v>
       </c>
@@ -39591,7 +39600,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="30">
+    <row r="19" spans="1:8" ht="30">
       <c r="A19" s="38" t="s">
         <v>1256</v>
       </c>
@@ -39614,7 +39623,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="27.75">
+    <row r="20" spans="1:8" ht="27.75">
       <c r="A20" s="38" t="s">
         <v>1260</v>
       </c>
@@ -39637,7 +39646,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="45">
+    <row r="21" spans="1:8" ht="45">
       <c r="A21" s="38" t="s">
         <v>1264</v>
       </c>
@@ -39660,7 +39669,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="30">
+    <row r="22" spans="1:8" ht="30">
       <c r="A22" s="38" t="s">
         <v>1267</v>
       </c>
@@ -39683,7 +39692,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="45">
+    <row r="23" spans="1:8" ht="45">
       <c r="A23" s="38" t="s">
         <v>1270</v>
       </c>
@@ -39706,7 +39715,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="45">
+    <row r="24" spans="1:8" ht="45">
       <c r="A24" s="38" t="s">
         <v>1273</v>
       </c>
@@ -39729,7 +39738,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="60">
+    <row r="25" spans="1:8" ht="60">
       <c r="A25" s="38" t="s">
         <v>1276</v>
       </c>
@@ -39752,7 +39761,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="42.75">
+    <row r="26" spans="1:8" ht="42.75">
       <c r="A26" s="38" t="s">
         <v>1279</v>
       </c>
@@ -39775,7 +39784,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="30">
+    <row r="27" spans="1:8" ht="30">
       <c r="A27" s="38" t="s">
         <v>1283</v>
       </c>
@@ -39798,7 +39807,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="45">
+    <row r="28" spans="1:8" ht="45">
       <c r="A28" s="38" t="s">
         <v>1287</v>
       </c>
@@ -39821,10 +39830,10 @@
         <v>407</v>
       </c>
       <c r="H28" s="38" t="s">
-        <v>1637</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="45">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="45">
       <c r="A29" s="38" t="s">
         <v>1290</v>
       </c>
@@ -39847,7 +39856,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="60">
+    <row r="30" spans="1:8" ht="60">
       <c r="A30" s="38" t="s">
         <v>1293</v>
       </c>
@@ -39869,23 +39878,11 @@
       <c r="G30" s="38" t="s">
         <v>407</v>
       </c>
-      <c r="I30" s="16" t="s">
-        <v>1651</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>1653</v>
-      </c>
-      <c r="K30" s="16" t="s">
-        <v>1654</v>
-      </c>
-      <c r="L30" s="16" t="s">
-        <v>1652</v>
-      </c>
-      <c r="M30" s="16" t="s">
-        <v>1655</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="60">
+      <c r="H30" s="67" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="60">
       <c r="A31" s="38" t="s">
         <v>1297</v>
       </c>
@@ -39907,11 +39904,11 @@
       <c r="G31" s="38" t="s">
         <v>407</v>
       </c>
-      <c r="I31" t="s">
-        <v>1656</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="60">
+      <c r="H31" s="67" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60">
       <c r="A32" s="38" t="s">
         <v>1301</v>
       </c>
@@ -39930,11 +39927,14 @@
       <c r="F32" s="38" t="s">
         <v>404</v>
       </c>
-      <c r="I32" t="s">
-        <v>1657</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="45">
+      <c r="G32" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="H32" s="67" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="45">
       <c r="A33" s="38" t="s">
         <v>1304</v>
       </c>
@@ -39950,8 +39950,17 @@
       <c r="E33" s="38" t="s">
         <v>1307</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="45">
+      <c r="F33" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="H33" s="67" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="45">
       <c r="A34" s="38" t="s">
         <v>1308</v>
       </c>
@@ -39967,8 +39976,32 @@
       <c r="E34" s="38" t="s">
         <v>1311</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="45">
+      <c r="F34" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="G34" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="H34" s="67" t="s">
+        <v>1658</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>1652</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>1654</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>1655</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>1653</v>
+      </c>
+      <c r="M34" s="16" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="45">
       <c r="A35" s="38" t="s">
         <v>1312</v>
       </c>
@@ -39984,8 +40017,17 @@
       <c r="E35" s="38" t="s">
         <v>1314</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="30">
+      <c r="F35" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="G35" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="H35" s="67" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="30">
       <c r="A36" s="38" t="s">
         <v>1315</v>
       </c>
@@ -40001,8 +40043,17 @@
       <c r="E36" s="38" t="s">
         <v>1317</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="30">
+      <c r="F36" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="G36" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="H36" s="67" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="30">
       <c r="A37" s="38" t="s">
         <v>1318</v>
       </c>
@@ -40018,8 +40069,17 @@
       <c r="E37" s="38" t="s">
         <v>1321</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="45">
+      <c r="F37" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="G37" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="H37" s="67" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="45">
       <c r="A38" s="38" t="s">
         <v>1322</v>
       </c>
@@ -40035,8 +40095,20 @@
       <c r="E38" s="38" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="45">
+      <c r="F38" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="G38" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="H38" s="67" t="s">
+        <v>1658</v>
+      </c>
+      <c r="I38" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="45">
       <c r="A39" s="38" t="s">
         <v>1326</v>
       </c>
@@ -40052,8 +40124,20 @@
       <c r="E39" s="38" t="s">
         <v>1329</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="45">
+      <c r="F39" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="G39" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="H39" s="67" t="s">
+        <v>1658</v>
+      </c>
+      <c r="I39" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="45">
       <c r="A40" s="38" t="s">
         <v>1330</v>
       </c>
@@ -40069,8 +40153,14 @@
       <c r="E40" s="38" t="s">
         <v>1332</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="45">
+      <c r="F40" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="G40" s="38" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="45">
       <c r="A41" s="38" t="s">
         <v>1333</v>
       </c>
@@ -40087,7 +40177,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="30">
+    <row r="42" spans="1:13" ht="30">
       <c r="A42" s="38" t="s">
         <v>1336</v>
       </c>

</xml_diff>

<commit_message>
chore: commit pending workspace changes
</commit_message>
<xml_diff>
--- a/tests/C2Pro_Test_Suites_Master.xlsx
+++ b/tests/C2Pro_Test_Suites_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esus_\Documents\AI\ZTWQ\c2pro\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6CCB49-8616-4C07-AF9D-87A7743B8679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3538C1-7E4B-4633-9A8E-494FC07C2B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12480" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2070" windowWidth="23280" windowHeight="12480" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suite Test" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5850" uniqueCount="1660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5897" uniqueCount="1704">
   <si>
     <t>Nº</t>
   </si>
@@ -12655,9 +12655,6 @@
   - test_i2_low_confidence_table_routes_to_human_review_conceptually</t>
   </si>
   <si>
-    <t>red</t>
-  </si>
-  <si>
     <t>detectado issue de seguridad</t>
   </si>
   <si>
@@ -12734,6 +12731,141 @@
   </si>
   <si>
     <t xml:space="preserve"> @qa-agent RED plan for S3-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1. [S3-12-RED-UNIT-01] Landmark semantics on core shell                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/accessibility/S3-12-landmarks.a11y.test.tsx       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: missing banner, navigation, main, or contentinfo roles.      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2. [S3-12-RED-UNIT-02] Heading hierarchy integrity                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/accessibility/S3-12-headings.a11y.test.tsx        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: skipped levels or non-linear heading order.                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  3. [S3-12-RED-UNIT-03] Control accessibility + focus-visible contract           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/accessibility/S3-12-controls.a11y.test.tsx        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: actionable controls lack accessible name or focus-visible    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     marker.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4. [S3-12-RED-UNIT-04] WCAG AA contrast threshold for critical text             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/accessibility/S3-12-contrast.a11y.test.tsx        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: contrast ratio for critical badge/text &lt; 4.5:1.              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  5. [S3-12-RED-UNIT-05] Modal focus trap + return-focus behavior                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/accessibility/S3-12-dialog-focus.a11y.test.tsx    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: focus escapes dialog or trigger focus is not restored on     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     close.                                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  6. [S3-12-RED-UNIT-06] Live region update discipline                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/accessibility/S3-12-live-regions.a11y.test.tsx    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: status not announced or duplicate spam on single transition. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  7. [S3-12-RED-INT-01] Axe critical violations gate (core shell)                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/integration/a11y/S3-12-axe-                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     critical.integration.test.tsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: endpoint unavailable or criticalViolations !== 0.            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  8. [S3-12-RED-INT-02] Keyboard traversal workflow integrity                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/integration/a11y/S3-12-keyboard-                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     flow.integration.test.tsx                                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: traps detected or workflow not completable by keyboard.      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  9. [S3-12-RED-INT-03] Tablet layout clipping/overlap checks                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/integration/responsive/S3-12-tablet-              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     layout.integration.test.tsx                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: clipped content or overlapping panels at 768x1024 and        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     820x1180.                                                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  10. [S3-12-RED-INT-04] Orientation-change state persistence                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: active context/state lost after portrait↔landscape switch.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  11. [S3-12-RED-INT-05] Reduced-motion + 200% zoom operability                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/integration/a11y/S3-12-accessibility-             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     modes.integration.test.tsx                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: mode toggles degrade readability/operability.                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  12. [S3-12-RED-E2E-01] Route-level a11y critical/blocker smoke                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/e2e/S3-12-a11y-tablet.spec.ts                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Fail condition: non-zero critical/blocker counters on dashboard route.       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  13. [S3-12-RED-E2E-02] Tablet portrait/landscape sanity on key flows            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Target: apps/web/src/tests/e2e/S3-12-a11y-tablet.spec.ts </t>
   </si>
 </sst>
 </file>
@@ -17593,8 +17725,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F264"/>
   <sheetViews>
-    <sheetView topLeftCell="A237" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A250" sqref="A250"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -18976,67 +19108,67 @@
     <row r="236" spans="2:2" hidden="1"/>
     <row r="243" spans="1:1">
       <c r="A243" s="16" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" s="16" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" s="16" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" s="16" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" s="16" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" s="16" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" s="16" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" s="16" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" s="16" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" s="16" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" s="16" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" s="16" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" s="16" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
   </sheetData>
@@ -39168,10 +39300,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -39179,7 +39311,7 @@
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.140625" bestFit="1" customWidth="1"/>
@@ -39830,7 +39962,7 @@
         <v>407</v>
       </c>
       <c r="H28" s="38" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="45">
@@ -39879,7 +40011,7 @@
         <v>407</v>
       </c>
       <c r="H30" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="60">
@@ -39905,7 +40037,7 @@
         <v>407</v>
       </c>
       <c r="H31" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="60">
@@ -39931,7 +40063,7 @@
         <v>407</v>
       </c>
       <c r="H32" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="45">
@@ -39957,7 +40089,7 @@
         <v>407</v>
       </c>
       <c r="H33" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="45">
@@ -39983,22 +40115,22 @@
         <v>407</v>
       </c>
       <c r="H34" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="I34" s="16" t="s">
+        <v>1651</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>1653</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>1654</v>
+      </c>
+      <c r="L34" s="16" t="s">
         <v>1652</v>
       </c>
-      <c r="J34" s="16" t="s">
-        <v>1654</v>
-      </c>
-      <c r="K34" s="16" t="s">
+      <c r="M34" s="16" t="s">
         <v>1655</v>
-      </c>
-      <c r="L34" s="16" t="s">
-        <v>1653</v>
-      </c>
-      <c r="M34" s="16" t="s">
-        <v>1656</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="45">
@@ -40024,7 +40156,7 @@
         <v>407</v>
       </c>
       <c r="H35" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="30">
@@ -40050,7 +40182,7 @@
         <v>407</v>
       </c>
       <c r="H36" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="30">
@@ -40076,7 +40208,7 @@
         <v>407</v>
       </c>
       <c r="H37" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="45">
@@ -40102,10 +40234,10 @@
         <v>407</v>
       </c>
       <c r="H38" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="I38" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="45">
@@ -40131,10 +40263,10 @@
         <v>407</v>
       </c>
       <c r="H39" s="67" t="s">
+        <v>1657</v>
+      </c>
+      <c r="I39" t="s">
         <v>1658</v>
-      </c>
-      <c r="I39" t="s">
-        <v>1659</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="45">
@@ -40157,7 +40289,7 @@
         <v>404</v>
       </c>
       <c r="G40" s="38" t="s">
-        <v>1637</v>
+        <v>407</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="45">
@@ -40192,6 +40324,241 @@
       </c>
       <c r="E42" s="38" t="s">
         <v>1338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="I44" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="I45" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="I46" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="I47" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="I48" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9">
+      <c r="I49" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9">
+      <c r="I50" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9">
+      <c r="I51" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9">
+      <c r="I52" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9">
+      <c r="I53" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9">
+      <c r="I54" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9">
+      <c r="I55" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9">
+      <c r="I56" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9">
+      <c r="I57" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9">
+      <c r="I58" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9">
+      <c r="I59" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9">
+      <c r="I60" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9">
+      <c r="I61" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="62" spans="9:9">
+      <c r="I62" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="63" spans="9:9">
+      <c r="I63" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="64" spans="9:9">
+      <c r="I64" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9">
+      <c r="I65" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9">
+      <c r="I66" t="s">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9">
+      <c r="I67" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9">
+      <c r="I68" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9">
+      <c r="I69" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="70" spans="9:9">
+      <c r="I70" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9">
+      <c r="I71" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="72" spans="9:9">
+      <c r="I72" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="73" spans="9:9">
+      <c r="I73" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="74" spans="9:9">
+      <c r="I74" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="75" spans="9:9">
+      <c r="I75" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="76" spans="9:9">
+      <c r="I76" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="77" spans="9:9">
+      <c r="I77" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="78" spans="9:9">
+      <c r="I78" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="79" spans="9:9">
+      <c r="I79" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="80" spans="9:9">
+      <c r="I80" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="81" spans="9:9">
+      <c r="I81" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="82" spans="9:9">
+      <c r="I82" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9">
+      <c r="I83" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9">
+      <c r="I84" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9">
+      <c r="I85" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9">
+      <c r="I86" t="s">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="87" spans="9:9">
+      <c r="I87" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="88" spans="9:9">
+      <c r="I88" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="89" spans="9:9">
+      <c r="I89" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="90" spans="9:9">
+      <c r="I90" t="s">
+        <v>1703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>